<commit_message>
visualization for directMerge added
</commit_message>
<xml_diff>
--- a/inputs/HeapSort_1.xlsx
+++ b/inputs/HeapSort_1.xlsx
@@ -14,17 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:si>
-    <x:t>Australia</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Oceania</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Canberra</x:t>
-  </x:si>
-</x:sst>
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -373,30 +363,12 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:E1"/>
+  <x:dimension ref="A1"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
-  <x:sheetData>
-    <x:row r="1" spans="1:5">
-      <x:c r="A1" s="0" t="s">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="B1" s="0" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="C1" s="0" t="s">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="D1" s="0">
-        <x:v>7692024</x:v>
-      </x:c>
-      <x:c r="E1" s="0">
-        <x:v>25687041</x:v>
-      </x:c>
-    </x:row>
-  </x:sheetData>
+  <x:sheetData/>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
   <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>

</xml_diff>